<commit_message>
Update readme. Add 2nd wireframe, update planning spreadsheet, add setup instructions
</commit_message>
<xml_diff>
--- a/planning/Favorite_Team.xlsx
+++ b/planning/Favorite_Team.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx37112/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554416CF-B33A-C448-A284-3CDC1F696813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7D1AA9-9A5E-A146-B9AF-27CE3D8128EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="2480" windowWidth="20120" windowHeight="16300" xr2:uid="{246DD3C1-5540-8343-9CEC-36BC19880D62}"/>
+    <workbookView xWindow="12740" yWindow="2860" windowWidth="20120" windowHeight="16300" xr2:uid="{246DD3C1-5540-8343-9CEC-36BC19880D62}"/>
   </bookViews>
   <sheets>
     <sheet name="favorite team" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="160">
   <si>
     <t>Teams</t>
   </si>
@@ -193,12 +193,6 @@
     <t>Chicago</t>
   </si>
   <si>
-    <t>background pictures, player detail page.</t>
-  </si>
-  <si>
-    <t>call to public API to get player stats or possibly team stats, multiple sports</t>
-  </si>
-  <si>
     <t>stat1</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
   </si>
   <si>
     <t>losses</t>
-  </si>
-  <si>
-    <t>as a sports fan I want to see deatails about a player</t>
   </si>
   <si>
     <t xml:space="preserve">    My Favorite Teams</t>
@@ -684,9 +675,6 @@
     <t>can the create method take an include</t>
   </si>
   <si>
-    <t>first test failed, but can reserch further if time allows.  Doc said to look at set</t>
-  </si>
-  <si>
     <t>set up team detail page</t>
   </si>
   <si>
@@ -730,6 +718,66 @@
   </si>
   <si>
     <t>player name</t>
+  </si>
+  <si>
+    <t>first test failed, but can reserch further if time allows.  Found documentation which said to look at set command</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>City:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> position</t>
+  </si>
+  <si>
+    <t>add additional fields to teams</t>
+  </si>
+  <si>
+    <t>add additional field to players</t>
+  </si>
+  <si>
+    <t>update seed data</t>
+  </si>
+  <si>
+    <t>deploy to heroku</t>
+  </si>
+  <si>
+    <t>reseed heroku</t>
+  </si>
+  <si>
+    <t>add delete to seed files</t>
+  </si>
+  <si>
+    <t>unseed all, seed all</t>
+  </si>
+  <si>
+    <t>background pictures, additional team and player fields.</t>
+  </si>
+  <si>
+    <t>player detail page.  call to public API to get player stats or possibly team stats, multiple sports</t>
+  </si>
+  <si>
+    <t>Possible future additions:</t>
+  </si>
+  <si>
+    <t>Could add a Player Detail page which shows some additonal stats about the player</t>
+  </si>
+  <si>
+    <t>SportDetails table to hold stats by sport and position.  It would be used to get stats that fit the players sport and positon.  For example, ERA, W, L for pitchers and BA, HR, RBI for position players.</t>
+  </si>
+  <si>
+    <t>API call to get current player stats</t>
+  </si>
+  <si>
+    <t>ability to update team or player once it is created</t>
   </si>
 </sst>
 </file>
@@ -1275,11 +1323,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B8CFAC-A0B2-F248-86D0-9D5BB67CEE19}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1299,10 +1345,10 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1339,13 +1385,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I4" t="s">
         <v>43</v>
@@ -1362,10 +1408,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
@@ -1377,10 +1423,10 @@
         <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1388,22 +1434,22 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1411,21 +1457,21 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
         <v>1</v>
@@ -1453,10 +1499,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L17" t="s">
         <v>42</v>
@@ -1589,7 +1635,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -1597,7 +1643,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
         <v>32</v>
@@ -1605,7 +1651,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -1620,17 +1666,37 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>78</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1643,31 +1709,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4504E8-1F2D-DE4C-B0B6-FFDF0DC818F3}">
-  <dimension ref="B2:K21"/>
+  <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="7"/>
       <c r="H3" s="4"/>
       <c r="I3" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -1678,25 +1746,25 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
       <c r="H5" s="11"/>
       <c r="I5" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
@@ -1705,14 +1773,14 @@
       <c r="F6" s="13"/>
       <c r="H6" s="11"/>
       <c r="I6" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1723,7 +1791,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12" t="s">
@@ -1733,12 +1801,12 @@
       <c r="F8" s="13"/>
       <c r="H8" s="11"/>
       <c r="I8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>16</v>
@@ -1755,7 +1823,7 @@
       </c>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -1766,64 +1834,64 @@
       <c r="J10" s="12"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F11" s="13"/>
       <c r="H11" s="11"/>
       <c r="I11" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F12" s="13"/>
       <c r="H12" s="11"/>
       <c r="I12" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F13" s="13"/>
       <c r="H13" s="11"/>
       <c r="I13" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1831,14 +1899,14 @@
       <c r="F14" s="13"/>
       <c r="H14" s="11"/>
       <c r="I14" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -1846,14 +1914,14 @@
       <c r="F15" s="13"/>
       <c r="H15" s="11"/>
       <c r="I15" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -1864,60 +1932,344 @@
       <c r="J16" s="12"/>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="17"/>
+    <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="20" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="7"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="M21" s="5"/>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="10"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B24" s="11"/>
+      <c r="D24" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="C26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H26" s="13"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" s="12"/>
+      <c r="N26" s="13"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B27" s="11"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="H27" s="13"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27" s="13"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M29" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="H30" s="13"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M30" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B31" s="11"/>
+      <c r="C31" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M31" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B32" s="11"/>
+      <c r="C32" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M32" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N32" s="13"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B33" s="11"/>
+      <c r="C33" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H33" s="13"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N33" s="13"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="13"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="13"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="13"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="13"/>
+    </row>
+    <row r="37" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1928,9 +2280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2233F8-3D30-C94C-9986-8D7CECC2F343}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1942,10 +2292,10 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1991,7 +2341,7 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
         <v>8</v>
@@ -2008,7 +2358,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
@@ -2040,7 +2390,7 @@
         <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2051,32 +2401,32 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
         <v>1</v>
@@ -2104,7 +2454,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -2118,7 +2468,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2137,7 +2487,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2148,7 +2498,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2159,7 +2509,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -2170,7 +2520,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -2178,7 +2528,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -2192,16 +2542,16 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" t="s">
         <v>74</v>
-      </c>
-      <c r="F21" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -2215,21 +2565,21 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
         <v>65</v>
-      </c>
-      <c r="G22" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2240,16 +2590,16 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2260,16 +2610,16 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -2280,16 +2630,16 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" t="s">
         <v>68</v>
-      </c>
-      <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2299,11 +2649,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBB64C3-2ADA-0448-BEDE-AC9F0D539291}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2313,203 +2661,236 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2521,9 +2902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3CF164-550D-9C49-A779-9EDA794CB87D}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2533,42 +2912,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
         <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>